<commit_message>
Renaming an R script, deleting outdated weather station metadata file, deleted battery voltage columns from weather station data.
</commit_message>
<xml_diff>
--- a/Stevens_et_al_2020/Data/Weather Stations/WeatherStationMetadata.xlsx
+++ b/Stevens_et_al_2020/Data/Weather Stations/WeatherStationMetadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katya/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/Berkeley/Post-Doc UCB/Research Projects/Fire-Water/Imagery Analysis/SEKI_Imagery_Analysis/Stevens_et_al_2020/Data/Weather Stations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C161D08C-07EE-2847-AFEA-43B0F636110E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ABA5E9-47FB-0A4E-A0A8-169DE8EDFD81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="3380" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{4F67C016-16B0-B54C-A055-B9250B272889}"/>
+    <workbookView xWindow="11560" yWindow="3380" windowWidth="27240" windowHeight="16440" xr2:uid="{4F67C016-16B0-B54C-A055-B9250B272889}"/>
   </bookViews>
   <sheets>
     <sheet name="File_and_Variable_Names" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>TIMESTAMP</t>
   </si>
@@ -40,12 +40,6 @@
     <t>RECORD</t>
   </si>
   <si>
-    <t>BattV_Min</t>
-  </si>
-  <si>
-    <t>BattV_TMn</t>
-  </si>
-  <si>
     <t>PTemp_C_Max</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>T_Avg</t>
   </si>
   <si>
-    <t>WS_ms</t>
-  </si>
-  <si>
     <t>WS_ms_Avg</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>datalogger record number</t>
   </si>
   <si>
-    <t>minimum battery voltage; Volts</t>
-  </si>
-  <si>
     <t>maximum battery temperatur; Deg C</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
   </si>
   <si>
     <t>time of maximum wind speed</t>
-  </si>
-  <si>
-    <t>time of minimum battery voltage</t>
   </si>
   <si>
     <t>time of maximum battery temperature</t>
@@ -608,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8D068A-F893-734D-A6AA-E9157DDCE717}">
-  <dimension ref="A3:E31"/>
+  <dimension ref="A3:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,109 +609,109 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -735,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -744,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -753,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -762,7 +747,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -771,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -780,150 +765,131 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="34" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="34" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="68" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
-      <c r="D18" t="s">
-        <v>14</v>
+      <c r="D18" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="34" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="68" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
-      <c r="D21" t="s">
-        <v>16</v>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="68" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
-      <c r="D22" t="s">
-        <v>17</v>
+      <c r="D22" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="68" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="34" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="68" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" ht="34" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="68" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" ht="68" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="34" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" ht="68" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>69</v>
+      <c r="D27" t="s">
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="3:5" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
-      <c r="D30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="C31" s="1"/>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>66</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -934,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83481DBD-9F12-4347-AB9E-BC2D0109F4BF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -943,7 +909,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="153" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>